<commit_message>
OpenApi - chat added to AI meal plan
</commit_message>
<xml_diff>
--- a/Daily_Work_Log_With_Day.xlsx
+++ b/Daily_Work_Log_With_Day.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loki/Desktop/GroceryGenius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD93367-793A-C341-BD60-453722CDF728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E964D7B4-6C24-E24E-BAE5-D0C52D7756B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Work Log" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date (Auto)</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>1.5hr</t>
+  </si>
+  <si>
+    <t>Added new liquid glass button features for smooth transision and also connected the project to GIT</t>
+  </si>
+  <si>
+    <t>2hr</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -407,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -440,18 +449,32 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <f ca="1">TODAY()</f>
         <v>45982</v>
       </c>
-      <c r="B2" s="1" t="str">
-        <f ca="1">TEXT(TODAY(), "dddd")</f>
-        <v>Friday</v>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <f ca="1">TODAY()</f>
+        <v>45983</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f ca="1">TEXT(TODAY(), "dddd")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>